<commit_message>
MTP080 generated, new code added to output list of orbits where a specific objective is measured
</commit_message>
<xml_diff>
--- a/nomad_mtp079_plan_generic.xlsx
+++ b/nomad_mtp079_plan_generic.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1983" uniqueCount="529">
   <si>
     <t>#orbitType</t>
   </si>
@@ -202,756 +202,762 @@
     <t>2024 APR 15 17:05:07</t>
   </si>
   <si>
+    <t>Surface 3SUBD #3</t>
+  </si>
+  <si>
+    <t>2024 APR 15 19:03:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:MERIDIANI SULPHATES; </t>
+  </si>
+  <si>
+    <t>2024 APR 15 21:01:03</t>
+  </si>
+  <si>
+    <t>2024 APR 15 22:59:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:EASTERN COPRATES; &amp;daysideMatch:COPRATES RISE; </t>
+  </si>
+  <si>
+    <t>2024 APR 16 00:56:58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=13.8hrs; &amp;Angle=25; </t>
+  </si>
+  <si>
+    <t>2024 APR 16 02:54:53</t>
+  </si>
+  <si>
+    <t>2024 APR 16 04:52:46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=13.7hrs; &amp;Angle=25; </t>
+  </si>
+  <si>
+    <t>2024 APR 16 06:50:42</t>
+  </si>
+  <si>
+    <t>2024 APR 16 08:48:42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=13.7hrs; &amp;Angle=24; </t>
+  </si>
+  <si>
+    <t>2024 APR 16 10:46:42</t>
+  </si>
+  <si>
+    <t>2024 APR 16 12:44:40</t>
+  </si>
+  <si>
+    <t>2024 APR 16 14:42:35</t>
+  </si>
+  <si>
+    <t>2024 APR 16 16:40:28</t>
+  </si>
+  <si>
+    <t>2024 APR 16 18:38:24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=13.6hrs; &amp;Angle=23; </t>
+  </si>
+  <si>
+    <t>2024 APR 16 20:36:22</t>
+  </si>
+  <si>
+    <t>2024 APR 16 22:34:21</t>
+  </si>
+  <si>
+    <t>2024 APR 17 00:32:19</t>
+  </si>
+  <si>
+    <t>Ice CO 2SUBD #2</t>
+  </si>
+  <si>
+    <t>2024 APR 17 02:30:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:CERAUNIUS THOLUS; &amp;mroOverlap; </t>
+  </si>
+  <si>
+    <t>2024 APR 17 04:28:07</t>
+  </si>
+  <si>
+    <t>2024 APR 17 06:26:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=13.6hrs; &amp;Angle=22; </t>
+  </si>
+  <si>
+    <t>2024 APR 17 08:24:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;trueNightLimb; </t>
+  </si>
+  <si>
+    <t>Ice CO 2SUBD #3</t>
+  </si>
+  <si>
+    <t>2024 APR 17 10:21:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:ELYSIUM MONS; </t>
+  </si>
+  <si>
+    <t>2024 APR 17 12:19:58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=13.5hrs; &amp;Angle=21; </t>
+  </si>
+  <si>
+    <t>2024 APR 17 14:17:53</t>
+  </si>
+  <si>
+    <t>2024 APR 17 16:15:46</t>
+  </si>
+  <si>
+    <t>2024 APR 17 18:13:40</t>
+  </si>
+  <si>
+    <t>2024 APR 17 20:11:38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=13.4hrs; &amp;Angle=20; </t>
+  </si>
+  <si>
+    <t>2024 APR 17 22:09:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:ACIDALIA MUD VOLCANOES NE; </t>
+  </si>
+  <si>
+    <t>2024 APR 18 00:07:34</t>
+  </si>
+  <si>
+    <t>2024 APR 18 02:05:30</t>
+  </si>
+  <si>
+    <t>2024 APR 18 04:03:24</t>
+  </si>
+  <si>
+    <t>2024 APR 18 06:01:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=13.4hrs; &amp;Angle=19; </t>
+  </si>
+  <si>
+    <t>2024 APR 18 07:59:14</t>
+  </si>
+  <si>
+    <t>2024 APR 18 09:57:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:CERBERUS FOSSAE; </t>
+  </si>
+  <si>
+    <t>2024 APR 18 11:55:13</t>
+  </si>
+  <si>
+    <t>2024 APR 18 13:53:10</t>
+  </si>
+  <si>
     <t>Ice H2O 2SUBD #1</t>
   </si>
   <si>
-    <t>2024 APR 15 19:03:04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:MERIDIANI SULPHATES; </t>
-  </si>
-  <si>
-    <t>2024 APR 15 21:01:03</t>
-  </si>
-  <si>
-    <t>2024 APR 15 22:59:01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:EASTERN COPRATES; &amp;daysideMatch:COPRATES RISE; </t>
-  </si>
-  <si>
-    <t>2024 APR 16 00:56:58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=13.8hrs; &amp;Angle=25; </t>
-  </si>
-  <si>
-    <t>2024 APR 16 02:54:53</t>
-  </si>
-  <si>
-    <t>2024 APR 16 04:52:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=13.7hrs; &amp;Angle=25; </t>
-  </si>
-  <si>
-    <t>2024 APR 16 06:50:42</t>
-  </si>
-  <si>
-    <t>2024 APR 16 08:48:42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=13.7hrs; &amp;Angle=24; </t>
-  </si>
-  <si>
-    <t>2024 APR 16 10:46:42</t>
-  </si>
-  <si>
-    <t>2024 APR 16 12:44:40</t>
-  </si>
-  <si>
-    <t>2024 APR 16 14:42:35</t>
-  </si>
-  <si>
-    <t>2024 APR 16 16:40:28</t>
-  </si>
-  <si>
-    <t>2024 APR 16 18:38:24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=13.6hrs; &amp;Angle=23; </t>
-  </si>
-  <si>
-    <t>2024 APR 16 20:36:22</t>
-  </si>
-  <si>
-    <t>2024 APR 16 22:34:21</t>
-  </si>
-  <si>
-    <t>2024 APR 17 00:32:19</t>
-  </si>
-  <si>
-    <t>Ice CO 2SUBD #2</t>
-  </si>
-  <si>
-    <t>2024 APR 17 02:30:14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:CERAUNIUS THOLUS; &amp;mroOverlap; </t>
-  </si>
-  <si>
-    <t>2024 APR 17 04:28:07</t>
-  </si>
-  <si>
-    <t>2024 APR 17 06:26:01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=13.6hrs; &amp;Angle=22; </t>
-  </si>
-  <si>
-    <t>2024 APR 17 08:24:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;trueNightLimb; </t>
+    <t>2024 APR 18 15:51:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:NILI FOSSAE; </t>
+  </si>
+  <si>
+    <t>2024 APR 18 17:48:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=13.3hrs; &amp;Angle=18; </t>
+  </si>
+  <si>
+    <t>2024 APR 18 19:46:53</t>
+  </si>
+  <si>
+    <t>2024 APR 18 21:44:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=13.2hrs; &amp;Angle=17; </t>
+  </si>
+  <si>
+    <t>2024 APR 18 23:42:49</t>
+  </si>
+  <si>
+    <t>2024 APR 19 01:40:46</t>
+  </si>
+  <si>
+    <t>2024 APR 19 03:38:40</t>
+  </si>
+  <si>
+    <t>2024 APR 19 05:36:32</t>
+  </si>
+  <si>
+    <t>6SUBD Nominal #53</t>
+  </si>
+  <si>
+    <t>2024 APR 19 07:34:27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;ingressMatch:PHOENIX; </t>
+  </si>
+  <si>
+    <t>2024 APR 19 09:32:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=13.2hrs; &amp;Angle=16; </t>
+  </si>
+  <si>
+    <t>2024 APR 19 11:30:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:CURIOSITY; </t>
+  </si>
+  <si>
+    <t>2024 APR 19 13:28:22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=13.1hrs; &amp;Angle=16; </t>
+  </si>
+  <si>
+    <t>2024 APR 19 15:26:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:UTOPIA; </t>
+  </si>
+  <si>
+    <t>2024 APR 19 17:24:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=13.1hrs; &amp;Angle=15; </t>
+  </si>
+  <si>
+    <t>2024 APR 19 19:22:04</t>
+  </si>
+  <si>
+    <t>2024 APR 19 21:20:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:VERNAL CRATER; </t>
+  </si>
+  <si>
+    <t>CH4 CO 2SUBD #3</t>
+  </si>
+  <si>
+    <t>2024 APR 19 23:18:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:ACIDALIA MUD VOLCANOES BASIN; </t>
+  </si>
+  <si>
+    <t>2024 APR 20 01:15:57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:EAST THAUMASIA; </t>
+  </si>
+  <si>
+    <t>2024 APR 20 03:13:53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=13.0hrs; &amp;Angle=14; </t>
+  </si>
+  <si>
+    <t>2024 APR 20 05:11:46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:ULYSSES THOLUS; &amp;daysideMatch:ARSIA MONS; </t>
+  </si>
+  <si>
+    <t>2024 APR 20 07:09:39</t>
+  </si>
+  <si>
+    <t>2024 APR 20 09:07:36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=13.0hrs; &amp;Angle=13; </t>
+  </si>
+  <si>
+    <t>2024 APR 20 11:05:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.9hrs; &amp;Angle=13; </t>
+  </si>
+  <si>
+    <t>2024 APR 20 13:03:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;possibleOCM; </t>
+  </si>
+  <si>
+    <t>2024 APR 20 15:01:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;possibleOCM; &amp;mroOverlap; </t>
+  </si>
+  <si>
+    <t>2024 APR 20 16:59:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.9hrs; &amp;Angle=12; </t>
+  </si>
+  <si>
+    <t>2024 APR 20 18:57:16</t>
+  </si>
+  <si>
+    <t>2024 APR 20 20:55:12</t>
+  </si>
+  <si>
+    <t>2024 APR 20 22:53:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:MAWRTH VALLIS-ARAM CHAOS; &amp;daysideMatch:MAWRTH VALLIS; </t>
+  </si>
+  <si>
+    <t>2024 APR 21 00:51:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.8hrs; &amp;Angle=12; </t>
+  </si>
+  <si>
+    <t>2024 APR 21 02:49:04</t>
+  </si>
+  <si>
+    <t>2024 APR 21 04:46:58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.8hrs; &amp;Angle=11; </t>
+  </si>
+  <si>
+    <t>2024 APR 21 06:44:50</t>
+  </si>
+  <si>
+    <t>6SUBD Nominal #12</t>
+  </si>
+  <si>
+    <t>2024 APR 21 08:42:45</t>
+  </si>
+  <si>
+    <t>2024 APR 21 10:40:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.8hrs; &amp;Angle=10; </t>
+  </si>
+  <si>
+    <t>2024 APR 21 12:38:43</t>
+  </si>
+  <si>
+    <t>2024 APR 21 14:36:40</t>
+  </si>
+  <si>
+    <t>2024 APR 21 16:34:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.7hrs; &amp;Angle=10; </t>
+  </si>
+  <si>
+    <t>2024 APR 21 18:32:27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;nomadPhobos; </t>
+  </si>
+  <si>
+    <t>2024 APR 21 20:30:22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.7hrs; &amp;Angle=9; </t>
+  </si>
+  <si>
+    <t>2024 APR 21 22:28:19</t>
+  </si>
+  <si>
+    <t>2024 APR 22 00:26:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.6hrs; &amp;Angle=9; </t>
+  </si>
+  <si>
+    <t>2024 APR 22 02:24:14</t>
+  </si>
+  <si>
+    <t>2024 APR 22 04:22:09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.6hrs; &amp;Angle=8; </t>
+  </si>
+  <si>
+    <t>2024 APR 22 06:20:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:ULYSSES FOSSAE; </t>
+  </si>
+  <si>
+    <t>2024 APR 22 08:17:55</t>
+  </si>
+  <si>
+    <t>2024 APR 22 10:15:52</t>
+  </si>
+  <si>
+    <t>2024 APR 22 12:13:51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.6hrs; &amp;Angle=7; </t>
+  </si>
+  <si>
+    <t>2024 APR 22 14:11:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.5hrs; &amp;Angle=7; </t>
+  </si>
+  <si>
+    <t>2024 APR 22 16:09:45</t>
+  </si>
+  <si>
+    <t>2024 APR 22 18:07:37</t>
+  </si>
+  <si>
+    <t>2024 APR 22 20:05:31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.5hrs; &amp;Angle=6; </t>
+  </si>
+  <si>
+    <t>2024 APR 22 22:03:27</t>
+  </si>
+  <si>
+    <t>2024 APR 23 00:01:25</t>
+  </si>
+  <si>
+    <t>2024 APR 23 01:59:22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.4hrs; &amp;Angle=6; </t>
+  </si>
+  <si>
+    <t>2024 APR 23 03:57:18</t>
+  </si>
+  <si>
+    <t>2024 APR 23 05:55:11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.4hrs; &amp;Angle=5; </t>
+  </si>
+  <si>
+    <t>2024 APR 23 07:53:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;nomadDeimos; </t>
+  </si>
+  <si>
+    <t>2024 APR 23 09:50:59</t>
+  </si>
+  <si>
+    <t>2024 APR 23 11:48:58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:ELYSIUM CERBERUS PHLEGRA; </t>
+  </si>
+  <si>
+    <t>2024 APR 23 13:46:57</t>
+  </si>
+  <si>
+    <t>2024 APR 23 15:44:54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.3hrs; &amp;Angle=4; </t>
+  </si>
+  <si>
+    <t>2024 APR 23 17:42:47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:PERSEVERANCE; </t>
+  </si>
+  <si>
+    <t>2024 APR 23 19:40:40</t>
+  </si>
+  <si>
+    <t>2024 APR 23 21:38:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.3hrs; &amp;Angle=3; </t>
+  </si>
+  <si>
+    <t>2024 APR 23 23:36:33</t>
+  </si>
+  <si>
+    <t>2024 APR 24 01:34:30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.2hrs; &amp;Angle=3; </t>
+  </si>
+  <si>
+    <t>2024 APR 24 03:32:27</t>
+  </si>
+  <si>
+    <t>2024 APR 24 05:30:21</t>
+  </si>
+  <si>
+    <t>2024 APR 24 07:28:13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.2hrs; &amp;Angle=2; </t>
+  </si>
+  <si>
+    <t>2024 APR 24 09:26:07</t>
+  </si>
+  <si>
+    <t>2024 APR 24 11:24:05</t>
+  </si>
+  <si>
+    <t>2024 APR 24 13:22:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.1hrs; &amp;Angle=2; </t>
+  </si>
+  <si>
+    <t>2024 APR 24 15:20:01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.1hrs; &amp;Angle=1; </t>
+  </si>
+  <si>
+    <t>2024 APR 24 17:17:56</t>
+  </si>
+  <si>
+    <t>2024 APR 24 19:15:48</t>
+  </si>
+  <si>
+    <t>2024 APR 24 21:13:41</t>
+  </si>
+  <si>
+    <t>2024 APR 24 23:11:38</t>
+  </si>
+  <si>
+    <t>2024 APR 25 01:09:35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:ARGYRE; </t>
+  </si>
+  <si>
+    <t>2024 APR 25 03:07:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=12.0hrs; &amp;Angle=0; </t>
+  </si>
+  <si>
+    <t>2024 APR 25 05:05:28</t>
+  </si>
+  <si>
+    <t>2024 APR 25 07:03:21</t>
+  </si>
+  <si>
+    <t>2024 APR 25 09:01:13</t>
+  </si>
+  <si>
+    <t>2024 APR 25 10:59:09</t>
+  </si>
+  <si>
+    <t>2024 APR 25 12:57:08</t>
+  </si>
+  <si>
+    <t>2024 APR 25 14:55:07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=11.9hrs; &amp;Angle=1; </t>
+  </si>
+  <si>
+    <t>2024 APR 25 16:53:03</t>
+  </si>
+  <si>
+    <t>2024 APR 25 18:50:56</t>
+  </si>
+  <si>
+    <t>2024 APR 25 20:48:48</t>
+  </si>
+  <si>
+    <t>2024 APR 25 22:46:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=11.9hrs; &amp;Angle=2; </t>
+  </si>
+  <si>
+    <t>2024 APR 26 00:44:41</t>
+  </si>
+  <si>
+    <t>2024 APR 26 02:42:38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=11.8hrs; &amp;Angle=2; </t>
+  </si>
+  <si>
+    <t>2024 APR 26 04:40:34</t>
+  </si>
+  <si>
+    <t>2024 APR 26 06:38:28</t>
+  </si>
+  <si>
+    <t>2024 APR 26 08:36:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=11.8hrs; &amp;Angle=3; </t>
+  </si>
+  <si>
+    <t>2024 APR 26 10:34:14</t>
+  </si>
+  <si>
+    <t>2024 APR 26 12:32:11</t>
+  </si>
+  <si>
+    <t>2024 APR 26 14:30:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=11.7hrs; &amp;Angle=3; </t>
+  </si>
+  <si>
+    <t>2024 APR 26 16:28:07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=11.7hrs; &amp;Angle=4; </t>
+  </si>
+  <si>
+    <t>2024 APR 26 18:26:01</t>
+  </si>
+  <si>
+    <t>2024 APR 26 20:23:53</t>
+  </si>
+  <si>
+    <t>2024 APR 26 22:21:46</t>
+  </si>
+  <si>
+    <t>2024 APR 27 00:19:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=11.7hrs; &amp;Angle=5; </t>
+  </si>
+  <si>
+    <t>2024 APR 27 02:17:40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=11.6hrs; &amp;Angle=5; </t>
+  </si>
+  <si>
+    <t>2024 APR 27 04:15:37</t>
+  </si>
+  <si>
+    <t>2024 APR 27 06:13:32</t>
+  </si>
+  <si>
+    <t>2024 APR 27 08:11:24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:OLYMPICA FOSSAE-JOVIS THOLUS; </t>
+  </si>
+  <si>
+    <t>2024 APR 27 10:09:16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=11.6hrs; &amp;Angle=6; </t>
+  </si>
+  <si>
+    <t>2024 APR 27 12:07:13</t>
+  </si>
+  <si>
+    <t>2024 APR 27 14:05:12</t>
+  </si>
+  <si>
+    <t>2024 APR 27 16:03:10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=11.5hrs; &amp;Angle=6; </t>
+  </si>
+  <si>
+    <t>2024 APR 27 18:01:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=11.5hrs; &amp;Angle=7; </t>
+  </si>
+  <si>
+    <t>2024 APR 27 19:58:58</t>
+  </si>
+  <si>
+    <t>2024 APR 27 21:56:50</t>
+  </si>
+  <si>
+    <t>2024 APR 27 23:54:46</t>
+  </si>
+  <si>
+    <t>2024 APR 28 01:52:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=11.4hrs; &amp;Angle=8; </t>
+  </si>
+  <si>
+    <t>2024 APR 28 03:50:40</t>
+  </si>
+  <si>
+    <t>2024 APR 28 05:48:35</t>
   </si>
   <si>
     <t>Surface Ice 2SUBD #1</t>
   </si>
   <si>
-    <t>2024 APR 17 10:21:59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:ELYSIUM MONS; </t>
-  </si>
-  <si>
-    <t>2024 APR 17 12:19:58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=13.5hrs; &amp;Angle=21; </t>
-  </si>
-  <si>
-    <t>2024 APR 17 14:17:53</t>
-  </si>
-  <si>
-    <t>2024 APR 17 16:15:46</t>
-  </si>
-  <si>
-    <t>2024 APR 17 18:13:40</t>
-  </si>
-  <si>
-    <t>2024 APR 17 20:11:38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=13.4hrs; &amp;Angle=20; </t>
-  </si>
-  <si>
-    <t>2024 APR 17 22:09:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:ACIDALIA MUD VOLCANOES NE; </t>
-  </si>
-  <si>
-    <t>2024 APR 18 00:07:34</t>
-  </si>
-  <si>
-    <t>2024 APR 18 02:05:30</t>
-  </si>
-  <si>
-    <t>2024 APR 18 04:03:24</t>
-  </si>
-  <si>
-    <t>2024 APR 18 06:01:17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=13.4hrs; &amp;Angle=19; </t>
-  </si>
-  <si>
-    <t>2024 APR 18 07:59:14</t>
+    <t>2024 APR 28 07:46:28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:ASCRAEUS MONS; </t>
+  </si>
+  <si>
+    <t>2024 APR 28 09:44:20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;daysideMatch:OLYMPUS MONS; </t>
+  </si>
+  <si>
+    <t>2024 APR 28 11:42:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=11.4hrs; &amp;Angle=9; </t>
+  </si>
+  <si>
+    <t>2024 APR 28 13:40:12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=11.3hrs; &amp;Angle=9; </t>
+  </si>
+  <si>
+    <t>2024 APR 28 15:38:10</t>
+  </si>
+  <si>
+    <t>2024 APR 28 17:36:07</t>
+  </si>
+  <si>
+    <t>2024 APR 28 19:34:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=11.3hrs; &amp;Angle=10; </t>
+  </si>
+  <si>
+    <t>2024 APR 28 21:31:52</t>
+  </si>
+  <si>
+    <t>2024 APR 28 23:29:46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;cassisSolarCalibration; </t>
+  </si>
+  <si>
+    <t>2024 APR 29 01:27:43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&amp;LST=11.2hrs; &amp;Angle=10; </t>
   </si>
   <si>
     <t>CH4 H2O 2SUBD 01</t>
   </si>
   <si>
-    <t>2024 APR 18 09:57:13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:CERBERUS FOSSAE; </t>
-  </si>
-  <si>
-    <t>2024 APR 18 11:55:13</t>
-  </si>
-  <si>
-    <t>2024 APR 18 13:53:10</t>
-  </si>
-  <si>
-    <t>2024 APR 18 15:51:04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:NILI FOSSAE; </t>
-  </si>
-  <si>
-    <t>2024 APR 18 17:48:57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=13.3hrs; &amp;Angle=18; </t>
-  </si>
-  <si>
-    <t>2024 APR 18 19:46:53</t>
-  </si>
-  <si>
-    <t>2024 APR 18 21:44:51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=13.2hrs; &amp;Angle=17; </t>
-  </si>
-  <si>
-    <t>2024 APR 18 23:42:49</t>
-  </si>
-  <si>
-    <t>2024 APR 19 01:40:46</t>
-  </si>
-  <si>
-    <t>2024 APR 19 03:38:40</t>
-  </si>
-  <si>
-    <t>2024 APR 19 05:36:32</t>
-  </si>
-  <si>
-    <t>6SUBD Nominal #42</t>
-  </si>
-  <si>
-    <t>2024 APR 19 07:34:27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;ingressMatch:PHOENIX; </t>
-  </si>
-  <si>
-    <t>2024 APR 19 09:32:25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=13.2hrs; &amp;Angle=16; </t>
-  </si>
-  <si>
-    <t>2024 APR 19 11:30:25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:CURIOSITY; </t>
-  </si>
-  <si>
-    <t>2024 APR 19 13:28:22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=13.1hrs; &amp;Angle=16; </t>
-  </si>
-  <si>
-    <t>2024 APR 19 15:26:17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:UTOPIA; </t>
-  </si>
-  <si>
-    <t>2024 APR 19 17:24:10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=13.1hrs; &amp;Angle=15; </t>
-  </si>
-  <si>
-    <t>2024 APR 19 19:22:04</t>
-  </si>
-  <si>
-    <t>2024 APR 19 21:20:01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:VERNAL CRATER; </t>
-  </si>
-  <si>
-    <t>2024 APR 19 23:18:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:ACIDALIA MUD VOLCANOES BASIN; </t>
-  </si>
-  <si>
-    <t>2024 APR 20 01:15:57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:EAST THAUMASIA; </t>
-  </si>
-  <si>
-    <t>2024 APR 20 03:13:53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=13.0hrs; &amp;Angle=14; </t>
-  </si>
-  <si>
-    <t>Ice CO 2SUBD #3</t>
-  </si>
-  <si>
-    <t>2024 APR 20 05:11:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:ULYSSES THOLUS; &amp;daysideMatch:ARSIA MONS; </t>
-  </si>
-  <si>
-    <t>2024 APR 20 07:09:39</t>
-  </si>
-  <si>
-    <t>2024 APR 20 09:07:36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=13.0hrs; &amp;Angle=13; </t>
-  </si>
-  <si>
-    <t>2024 APR 20 11:05:35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.9hrs; &amp;Angle=13; </t>
-  </si>
-  <si>
-    <t>2024 APR 20 13:03:34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;possibleOCM; </t>
-  </si>
-  <si>
-    <t>2024 APR 20 15:01:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;possibleOCM; &amp;mroOverlap; </t>
-  </si>
-  <si>
-    <t>2024 APR 20 16:59:23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.9hrs; &amp;Angle=12; </t>
-  </si>
-  <si>
-    <t>2024 APR 20 18:57:16</t>
-  </si>
-  <si>
-    <t>2024 APR 20 20:55:12</t>
-  </si>
-  <si>
-    <t>2024 APR 20 22:53:10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:MAWRTH VALLIS-ARAM CHAOS; &amp;daysideMatch:MAWRTH VALLIS; </t>
-  </si>
-  <si>
-    <t>2024 APR 21 00:51:08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.8hrs; &amp;Angle=12; </t>
-  </si>
-  <si>
-    <t>2024 APR 21 02:49:04</t>
-  </si>
-  <si>
-    <t>2024 APR 21 04:46:58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.8hrs; &amp;Angle=11; </t>
-  </si>
-  <si>
-    <t>2024 APR 21 06:44:50</t>
-  </si>
-  <si>
-    <t>6SUBD Nominal #48</t>
-  </si>
-  <si>
-    <t>2024 APR 21 08:42:45</t>
-  </si>
-  <si>
-    <t>2024 APR 21 10:40:43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.8hrs; &amp;Angle=10; </t>
-  </si>
-  <si>
-    <t>2024 APR 21 12:38:43</t>
-  </si>
-  <si>
-    <t>2024 APR 21 14:36:40</t>
-  </si>
-  <si>
-    <t>2024 APR 21 16:34:34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.7hrs; &amp;Angle=10; </t>
-  </si>
-  <si>
-    <t>2024 APR 21 18:32:27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;nomadPhobos; </t>
-  </si>
-  <si>
-    <t>2024 APR 21 20:30:22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.7hrs; &amp;Angle=9; </t>
-  </si>
-  <si>
-    <t>2024 APR 21 22:28:19</t>
-  </si>
-  <si>
-    <t>2024 APR 22 00:26:17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.6hrs; &amp;Angle=9; </t>
-  </si>
-  <si>
-    <t>2024 APR 22 02:24:14</t>
-  </si>
-  <si>
-    <t>2024 APR 22 04:22:09</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.6hrs; &amp;Angle=8; </t>
-  </si>
-  <si>
-    <t>2024 APR 22 06:20:01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:ULYSSES FOSSAE; </t>
-  </si>
-  <si>
-    <t>2024 APR 22 08:17:55</t>
-  </si>
-  <si>
-    <t>2024 APR 22 10:15:52</t>
-  </si>
-  <si>
-    <t>2024 APR 22 12:13:51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.6hrs; &amp;Angle=7; </t>
-  </si>
-  <si>
-    <t>2024 APR 22 14:11:50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.5hrs; &amp;Angle=7; </t>
-  </si>
-  <si>
-    <t>2024 APR 22 16:09:45</t>
-  </si>
-  <si>
-    <t>2024 APR 22 18:07:37</t>
-  </si>
-  <si>
-    <t>2024 APR 22 20:05:31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.5hrs; &amp;Angle=6; </t>
-  </si>
-  <si>
-    <t>2024 APR 22 22:03:27</t>
-  </si>
-  <si>
-    <t>2024 APR 23 00:01:25</t>
-  </si>
-  <si>
-    <t>2024 APR 23 01:59:22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.4hrs; &amp;Angle=6; </t>
-  </si>
-  <si>
-    <t>2024 APR 23 03:57:18</t>
-  </si>
-  <si>
-    <t>2024 APR 23 05:55:11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.4hrs; &amp;Angle=5; </t>
-  </si>
-  <si>
-    <t>2024 APR 23 07:53:03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;nomadDeimos; </t>
-  </si>
-  <si>
-    <t>2024 APR 23 09:50:59</t>
-  </si>
-  <si>
-    <t>2024 APR 23 11:48:58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:ELYSIUM CERBERUS PHLEGRA; </t>
-  </si>
-  <si>
-    <t>2024 APR 23 13:46:57</t>
-  </si>
-  <si>
-    <t>2024 APR 23 15:44:54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.3hrs; &amp;Angle=4; </t>
-  </si>
-  <si>
-    <t>2024 APR 23 17:42:47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:PERSEVERANCE; </t>
-  </si>
-  <si>
-    <t>2024 APR 23 19:40:40</t>
-  </si>
-  <si>
-    <t>2024 APR 23 21:38:35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.3hrs; &amp;Angle=3; </t>
-  </si>
-  <si>
-    <t>2024 APR 23 23:36:33</t>
-  </si>
-  <si>
-    <t>2024 APR 24 01:34:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.2hrs; &amp;Angle=3; </t>
-  </si>
-  <si>
-    <t>2024 APR 24 03:32:27</t>
-  </si>
-  <si>
-    <t>2024 APR 24 05:30:21</t>
-  </si>
-  <si>
-    <t>2024 APR 24 07:28:13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.2hrs; &amp;Angle=2; </t>
-  </si>
-  <si>
-    <t>2024 APR 24 09:26:07</t>
-  </si>
-  <si>
-    <t>2024 APR 24 11:24:05</t>
-  </si>
-  <si>
-    <t>2024 APR 24 13:22:04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.1hrs; &amp;Angle=2; </t>
-  </si>
-  <si>
-    <t>2024 APR 24 15:20:01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.1hrs; &amp;Angle=1; </t>
-  </si>
-  <si>
-    <t>2024 APR 24 17:17:56</t>
-  </si>
-  <si>
-    <t>2024 APR 24 19:15:48</t>
-  </si>
-  <si>
-    <t>2024 APR 24 21:13:41</t>
-  </si>
-  <si>
-    <t>2024 APR 24 23:11:38</t>
-  </si>
-  <si>
-    <t>2024 APR 25 01:09:35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:ARGYRE; </t>
-  </si>
-  <si>
-    <t>2024 APR 25 03:07:33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=12.0hrs; &amp;Angle=0; </t>
-  </si>
-  <si>
-    <t>2024 APR 25 05:05:28</t>
-  </si>
-  <si>
-    <t>2024 APR 25 07:03:21</t>
-  </si>
-  <si>
-    <t>2024 APR 25 09:01:13</t>
-  </si>
-  <si>
-    <t>2024 APR 25 10:59:09</t>
-  </si>
-  <si>
-    <t>2024 APR 25 12:57:08</t>
-  </si>
-  <si>
-    <t>2024 APR 25 14:55:07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=11.9hrs; &amp;Angle=1; </t>
-  </si>
-  <si>
-    <t>2024 APR 25 16:53:03</t>
-  </si>
-  <si>
-    <t>2024 APR 25 18:50:56</t>
-  </si>
-  <si>
-    <t>2024 APR 25 20:48:48</t>
-  </si>
-  <si>
-    <t>2024 APR 25 22:46:44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=11.9hrs; &amp;Angle=2; </t>
-  </si>
-  <si>
-    <t>2024 APR 26 00:44:41</t>
-  </si>
-  <si>
-    <t>2024 APR 26 02:42:38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=11.8hrs; &amp;Angle=2; </t>
-  </si>
-  <si>
-    <t>2024 APR 26 04:40:34</t>
-  </si>
-  <si>
-    <t>2024 APR 26 06:38:28</t>
-  </si>
-  <si>
-    <t>2024 APR 26 08:36:20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=11.8hrs; &amp;Angle=3; </t>
-  </si>
-  <si>
-    <t>2024 APR 26 10:34:14</t>
-  </si>
-  <si>
-    <t>2024 APR 26 12:32:11</t>
-  </si>
-  <si>
-    <t>2024 APR 26 14:30:10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=11.7hrs; &amp;Angle=3; </t>
-  </si>
-  <si>
-    <t>2024 APR 26 16:28:07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=11.7hrs; &amp;Angle=4; </t>
-  </si>
-  <si>
-    <t>2024 APR 26 18:26:01</t>
-  </si>
-  <si>
-    <t>2024 APR 26 20:23:53</t>
-  </si>
-  <si>
-    <t>2024 APR 26 22:21:46</t>
-  </si>
-  <si>
-    <t>2024 APR 27 00:19:43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=11.7hrs; &amp;Angle=5; </t>
-  </si>
-  <si>
-    <t>2024 APR 27 02:17:40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=11.6hrs; &amp;Angle=5; </t>
-  </si>
-  <si>
-    <t>2024 APR 27 04:15:37</t>
-  </si>
-  <si>
-    <t>2024 APR 27 06:13:32</t>
-  </si>
-  <si>
-    <t>2024 APR 27 08:11:24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:OLYMPICA FOSSAE-JOVIS THOLUS; </t>
-  </si>
-  <si>
-    <t>2024 APR 27 10:09:16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=11.6hrs; &amp;Angle=6; </t>
-  </si>
-  <si>
-    <t>2024 APR 27 12:07:13</t>
-  </si>
-  <si>
-    <t>2024 APR 27 14:05:12</t>
-  </si>
-  <si>
-    <t>2024 APR 27 16:03:10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=11.5hrs; &amp;Angle=6; </t>
-  </si>
-  <si>
-    <t>2024 APR 27 18:01:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=11.5hrs; &amp;Angle=7; </t>
-  </si>
-  <si>
-    <t>2024 APR 27 19:58:58</t>
-  </si>
-  <si>
-    <t>2024 APR 27 21:56:50</t>
-  </si>
-  <si>
-    <t>2024 APR 27 23:54:46</t>
-  </si>
-  <si>
-    <t>2024 APR 28 01:52:43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=11.4hrs; &amp;Angle=8; </t>
-  </si>
-  <si>
-    <t>2024 APR 28 03:50:40</t>
-  </si>
-  <si>
-    <t>2024 APR 28 05:48:35</t>
-  </si>
-  <si>
-    <t>2024 APR 28 07:46:28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:ASCRAEUS MONS; </t>
-  </si>
-  <si>
-    <t>2024 APR 28 09:44:20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;daysideMatch:OLYMPUS MONS; </t>
-  </si>
-  <si>
-    <t>2024 APR 28 11:42:14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=11.4hrs; &amp;Angle=9; </t>
-  </si>
-  <si>
-    <t>2024 APR 28 13:40:12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=11.3hrs; &amp;Angle=9; </t>
-  </si>
-  <si>
-    <t>2024 APR 28 15:38:10</t>
-  </si>
-  <si>
-    <t>2024 APR 28 17:36:07</t>
-  </si>
-  <si>
-    <t>2024 APR 28 19:34:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=11.3hrs; &amp;Angle=10; </t>
-  </si>
-  <si>
-    <t>2024 APR 28 21:31:52</t>
-  </si>
-  <si>
-    <t>2024 APR 28 23:29:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;cassisSolarCalibration; </t>
-  </si>
-  <si>
-    <t>2024 APR 29 01:27:43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&amp;LST=11.2hrs; &amp;Angle=10; </t>
-  </si>
-  <si>
     <t>2024 APR 29 03:25:40</t>
   </si>
   <si>
@@ -1006,9 +1012,6 @@
     <t xml:space="preserve">&amp;LST=11.0hrs; &amp;Angle=13; </t>
   </si>
   <si>
-    <t>Surface 3SUBD #3</t>
-  </si>
-  <si>
     <t>2024 APR 30 03:00:40</t>
   </si>
   <si>
@@ -1307,9 +1310,6 @@
   </si>
   <si>
     <t xml:space="preserve">&amp;LST=9.8hrs; &amp;Angle=30; </t>
-  </si>
-  <si>
-    <t>CH4 CO 2SUBD #3</t>
   </si>
   <si>
     <t>2024 MAY 05 22:32:32</t>
@@ -3369,16 +3369,16 @@
         <v>3</v>
       </c>
       <c r="H60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I60" t="s">
+        <v>8</v>
+      </c>
+      <c r="L60" t="s">
         <v>111</v>
       </c>
-      <c r="I60" t="s">
-        <v>8</v>
-      </c>
-      <c r="L60" t="s">
+      <c r="M60" t="s">
         <v>112</v>
-      </c>
-      <c r="M60" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:13">
@@ -3401,7 +3401,7 @@
         <v>8</v>
       </c>
       <c r="L61" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M61" t="s">
         <v>28</v>
@@ -3418,7 +3418,7 @@
         <v>8</v>
       </c>
       <c r="L62" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M62" t="s">
         <v>28</v>
@@ -3438,7 +3438,7 @@
         <v>6</v>
       </c>
       <c r="H63" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="I63" t="s">
         <v>8</v>
@@ -3638,7 +3638,7 @@
         <v>3</v>
       </c>
       <c r="H73" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="I73" t="s">
         <v>8</v>
@@ -3681,7 +3681,7 @@
         <v>3</v>
       </c>
       <c r="H75" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="I75" t="s">
         <v>8</v>
@@ -3770,16 +3770,16 @@
         <v>6</v>
       </c>
       <c r="H79" t="s">
-        <v>24</v>
+        <v>143</v>
       </c>
       <c r="I79" t="s">
         <v>8</v>
       </c>
       <c r="L79" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="M79" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="80" spans="1:13">
@@ -3793,10 +3793,10 @@
         <v>8</v>
       </c>
       <c r="L80" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M80" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="81" spans="1:13">
@@ -3819,10 +3819,10 @@
         <v>8</v>
       </c>
       <c r="L81" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="M81" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="82" spans="1:13">
@@ -3839,7 +3839,7 @@
         <v>3</v>
       </c>
       <c r="H82" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="I82" t="s">
         <v>8</v>
@@ -3862,7 +3862,7 @@
         <v>152</v>
       </c>
       <c r="M83" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="1:13">
@@ -3998,7 +3998,7 @@
         <v>6</v>
       </c>
       <c r="H91" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="I91" t="s">
         <v>8</v>
@@ -4447,16 +4447,22 @@
     </row>
     <row r="113" spans="1:13">
       <c r="A113">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="I113" t="s">
         <v>8</v>
+      </c>
+      <c r="J113" t="s">
+        <v>29</v>
+      </c>
+      <c r="K113" t="s">
+        <v>30</v>
       </c>
       <c r="L113" t="s">
         <v>200</v>
       </c>
       <c r="M113" t="s">
-        <v>198</v>
+        <v>92</v>
       </c>
     </row>
     <row r="114" spans="1:13">
@@ -4553,7 +4559,7 @@
         <v>6</v>
       </c>
       <c r="H118" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="I118" t="s">
         <v>8</v>
@@ -5008,7 +5014,7 @@
         <v>3</v>
       </c>
       <c r="H140" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="I140" t="s">
         <v>8</v>
@@ -5612,7 +5618,7 @@
         <v>3</v>
       </c>
       <c r="H169" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="I169" t="s">
         <v>8</v>
@@ -5834,16 +5840,16 @@
         <v>3</v>
       </c>
       <c r="H181" t="s">
-        <v>93</v>
+        <v>295</v>
       </c>
       <c r="I181" t="s">
         <v>8</v>
       </c>
       <c r="L181" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="M181" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="182" spans="1:13">
@@ -5851,16 +5857,16 @@
         <v>3</v>
       </c>
       <c r="H182" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="I182" t="s">
         <v>8</v>
       </c>
       <c r="L182" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M182" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="183" spans="1:13">
@@ -5883,10 +5889,10 @@
         <v>8</v>
       </c>
       <c r="L183" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="M183" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="184" spans="1:13">
@@ -5909,10 +5915,10 @@
         <v>8</v>
       </c>
       <c r="L184" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="M184" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="185" spans="1:13">
@@ -5926,7 +5932,7 @@
         <v>8</v>
       </c>
       <c r="L185" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M185" t="s">
         <v>133</v>
@@ -5952,7 +5958,7 @@
         <v>8</v>
       </c>
       <c r="L186" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="M186" t="s">
         <v>28</v>
@@ -5966,10 +5972,10 @@
         <v>8</v>
       </c>
       <c r="L187" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="M187" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="188" spans="1:13">
@@ -5992,10 +5998,10 @@
         <v>8</v>
       </c>
       <c r="L188" t="s">
+        <v>308</v>
+      </c>
+      <c r="M188" t="s">
         <v>307</v>
-      </c>
-      <c r="M188" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="189" spans="1:13">
@@ -6003,10 +6009,10 @@
         <v>14</v>
       </c>
       <c r="L189" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M189" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="190" spans="1:13">
@@ -6020,10 +6026,10 @@
         <v>8</v>
       </c>
       <c r="L190" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="M190" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="191" spans="1:13">
@@ -6040,16 +6046,16 @@
         <v>6</v>
       </c>
       <c r="H191" t="s">
-        <v>24</v>
+        <v>313</v>
       </c>
       <c r="I191" t="s">
         <v>8</v>
       </c>
       <c r="L191" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="M191" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="192" spans="1:13">
@@ -6072,10 +6078,10 @@
         <v>8</v>
       </c>
       <c r="L192" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="M192" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="193" spans="1:13">
@@ -6089,10 +6095,10 @@
         <v>8</v>
       </c>
       <c r="L193" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="M193" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="194" spans="1:13">
@@ -6109,16 +6115,16 @@
         <v>3</v>
       </c>
       <c r="H194" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="I194" t="s">
         <v>8</v>
       </c>
       <c r="L194" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="M194" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="195" spans="1:13">
@@ -6129,10 +6135,10 @@
         <v>8</v>
       </c>
       <c r="L195" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="M195" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="196" spans="1:13">
@@ -6155,10 +6161,10 @@
         <v>8</v>
       </c>
       <c r="L196" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="M196" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="197" spans="1:13">
@@ -6181,10 +6187,10 @@
         <v>8</v>
       </c>
       <c r="L197" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="M197" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="198" spans="1:13">
@@ -6195,10 +6201,10 @@
         <v>8</v>
       </c>
       <c r="L198" t="s">
+        <v>325</v>
+      </c>
+      <c r="M198" t="s">
         <v>323</v>
-      </c>
-      <c r="M198" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="199" spans="1:13">
@@ -6221,10 +6227,10 @@
         <v>8</v>
       </c>
       <c r="L199" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="M199" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="200" spans="1:13">
@@ -6235,10 +6241,10 @@
         <v>8</v>
       </c>
       <c r="L200" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="M200" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="201" spans="1:13">
@@ -6261,10 +6267,10 @@
         <v>8</v>
       </c>
       <c r="L201" t="s">
+        <v>329</v>
+      </c>
+      <c r="M201" t="s">
         <v>327</v>
-      </c>
-      <c r="M201" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="202" spans="1:13">
@@ -6287,10 +6293,10 @@
         <v>8</v>
       </c>
       <c r="L202" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="M202" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="203" spans="1:13">
@@ -6298,13 +6304,13 @@
         <v>3</v>
       </c>
       <c r="H203" t="s">
-        <v>330</v>
+        <v>85</v>
       </c>
       <c r="I203" t="s">
         <v>8</v>
       </c>
       <c r="L203" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="M203" t="s">
         <v>166</v>
@@ -6330,10 +6336,10 @@
         <v>8</v>
       </c>
       <c r="L204" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="M204" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="205" spans="1:13">
@@ -6347,7 +6353,7 @@
         <v>8</v>
       </c>
       <c r="L205" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="M205" t="s">
         <v>28</v>
@@ -6373,10 +6379,10 @@
         <v>8</v>
       </c>
       <c r="L206" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="M206" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="207" spans="1:13">
@@ -6387,10 +6393,10 @@
         <v>8</v>
       </c>
       <c r="L207" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="M207" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="208" spans="1:13">
@@ -6413,10 +6419,10 @@
         <v>8</v>
       </c>
       <c r="L208" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="M208" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="209" spans="1:13">
@@ -6439,10 +6445,10 @@
         <v>8</v>
       </c>
       <c r="L209" t="s">
+        <v>341</v>
+      </c>
+      <c r="M209" t="s">
         <v>340</v>
-      </c>
-      <c r="M209" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="210" spans="1:13">
@@ -6456,7 +6462,7 @@
         <v>8</v>
       </c>
       <c r="L210" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="M210" t="s">
         <v>38</v>
@@ -6482,7 +6488,7 @@
         <v>8</v>
       </c>
       <c r="L211" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="M211" t="s">
         <v>40</v>
@@ -6496,10 +6502,10 @@
         <v>8</v>
       </c>
       <c r="L212" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="M212" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="213" spans="1:13">
@@ -6522,10 +6528,10 @@
         <v>8</v>
       </c>
       <c r="L213" t="s">
+        <v>346</v>
+      </c>
+      <c r="M213" t="s">
         <v>345</v>
-      </c>
-      <c r="M213" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="214" spans="1:13">
@@ -6536,10 +6542,10 @@
         <v>8</v>
       </c>
       <c r="L214" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="M214" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="215" spans="1:13">
@@ -6562,10 +6568,10 @@
         <v>8</v>
       </c>
       <c r="L215" t="s">
+        <v>349</v>
+      </c>
+      <c r="M215" t="s">
         <v>348</v>
-      </c>
-      <c r="M215" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="216" spans="1:13">
@@ -6588,10 +6594,10 @@
         <v>8</v>
       </c>
       <c r="L216" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="M216" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="217" spans="1:13">
@@ -6602,10 +6608,10 @@
         <v>8</v>
       </c>
       <c r="L217" t="s">
+        <v>352</v>
+      </c>
+      <c r="M217" t="s">
         <v>351</v>
-      </c>
-      <c r="M217" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="218" spans="1:13">
@@ -6616,10 +6622,10 @@
         <v>8</v>
       </c>
       <c r="L218" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="M218" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="219" spans="1:13">
@@ -6642,10 +6648,10 @@
         <v>8</v>
       </c>
       <c r="L219" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="M219" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="220" spans="1:13">
@@ -6656,10 +6662,10 @@
         <v>8</v>
       </c>
       <c r="L220" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="M220" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="221" spans="1:13">
@@ -6682,10 +6688,10 @@
         <v>8</v>
       </c>
       <c r="L221" t="s">
+        <v>357</v>
+      </c>
+      <c r="M221" t="s">
         <v>356</v>
-      </c>
-      <c r="M221" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="222" spans="1:13">
@@ -6708,10 +6714,10 @@
         <v>8</v>
       </c>
       <c r="L222" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="M222" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="223" spans="1:13">
@@ -6722,10 +6728,10 @@
         <v>8</v>
       </c>
       <c r="L223" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="M223" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="224" spans="1:13">
@@ -6748,10 +6754,10 @@
         <v>8</v>
       </c>
       <c r="L224" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="M224" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="225" spans="1:13">
@@ -6762,10 +6768,10 @@
         <v>8</v>
       </c>
       <c r="L225" t="s">
+        <v>363</v>
+      </c>
+      <c r="M225" t="s">
         <v>362</v>
-      </c>
-      <c r="M225" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="226" spans="1:13">
@@ -6788,10 +6794,10 @@
         <v>8</v>
       </c>
       <c r="L226" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="M226" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="227" spans="1:13">
@@ -6808,7 +6814,7 @@
         <v>30</v>
       </c>
       <c r="L227" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="M227" t="s">
         <v>92</v>
@@ -6834,10 +6840,10 @@
         <v>8</v>
       </c>
       <c r="L228" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="M228" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="229" spans="1:13">
@@ -6845,16 +6851,16 @@
         <v>3</v>
       </c>
       <c r="H229" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="I229" t="s">
         <v>8</v>
       </c>
       <c r="L229" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="M229" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
     </row>
     <row r="230" spans="1:13">
@@ -6862,13 +6868,13 @@
         <v>3</v>
       </c>
       <c r="H230" t="s">
-        <v>24</v>
+        <v>313</v>
       </c>
       <c r="I230" t="s">
         <v>8</v>
       </c>
       <c r="L230" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="M230" t="s">
         <v>26</v>
@@ -6894,10 +6900,10 @@
         <v>8</v>
       </c>
       <c r="L231" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="M231" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="232" spans="1:13">
@@ -6908,10 +6914,10 @@
         <v>8</v>
       </c>
       <c r="L232" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="M232" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
     </row>
     <row r="233" spans="1:13">
@@ -6919,7 +6925,7 @@
         <v>14</v>
       </c>
       <c r="L233" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="M233" t="s">
         <v>182</v>
@@ -6954,10 +6960,10 @@
         <v>8</v>
       </c>
       <c r="L234" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="M234" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="235" spans="1:13">
@@ -6968,10 +6974,10 @@
         <v>8</v>
       </c>
       <c r="L235" t="s">
+        <v>379</v>
+      </c>
+      <c r="M235" t="s">
         <v>378</v>
-      </c>
-      <c r="M235" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="236" spans="1:13">
@@ -7003,10 +7009,10 @@
         <v>8</v>
       </c>
       <c r="L236" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="M236" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="237" spans="1:13">
@@ -7038,7 +7044,7 @@
         <v>8</v>
       </c>
       <c r="L237" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="M237" t="s">
         <v>219</v>
@@ -7052,10 +7058,10 @@
         <v>8</v>
       </c>
       <c r="L238" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="M238" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="239" spans="1:13">
@@ -7066,10 +7072,10 @@
         <v>8</v>
       </c>
       <c r="L239" t="s">
+        <v>384</v>
+      </c>
+      <c r="M239" t="s">
         <v>383</v>
-      </c>
-      <c r="M239" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="240" spans="1:13">
@@ -7101,10 +7107,10 @@
         <v>8</v>
       </c>
       <c r="L240" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="M240" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="241" spans="1:13">
@@ -7118,7 +7124,7 @@
         <v>8</v>
       </c>
       <c r="L241" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="M241" t="s">
         <v>28</v>
@@ -7144,10 +7150,10 @@
         <v>8</v>
       </c>
       <c r="L242" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="M242" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="243" spans="1:13">
@@ -7158,10 +7164,10 @@
         <v>8</v>
       </c>
       <c r="L243" t="s">
+        <v>389</v>
+      </c>
+      <c r="M243" t="s">
         <v>388</v>
-      </c>
-      <c r="M243" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="244" spans="1:13">
@@ -7193,10 +7199,10 @@
         <v>8</v>
       </c>
       <c r="L244" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="M244" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="245" spans="1:13">
@@ -7204,7 +7210,7 @@
         <v>14</v>
       </c>
       <c r="L245" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="M245" t="s">
         <v>182</v>
@@ -7239,10 +7245,10 @@
         <v>8</v>
       </c>
       <c r="L246" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="M246" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="247" spans="1:13">
@@ -7253,10 +7259,10 @@
         <v>8</v>
       </c>
       <c r="L247" t="s">
+        <v>395</v>
+      </c>
+      <c r="M247" t="s">
         <v>394</v>
-      </c>
-      <c r="M247" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="248" spans="1:13">
@@ -7288,10 +7294,10 @@
         <v>8</v>
       </c>
       <c r="L248" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="M248" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="249" spans="1:13">
@@ -7302,10 +7308,10 @@
         <v>8</v>
       </c>
       <c r="L249" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="M249" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="250" spans="1:13">
@@ -7337,10 +7343,10 @@
         <v>8</v>
       </c>
       <c r="L250" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M250" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="251" spans="1:13">
@@ -7357,7 +7363,7 @@
         <v>30</v>
       </c>
       <c r="L251" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="M251" t="s">
         <v>92</v>
@@ -7386,13 +7392,13 @@
         <v>6</v>
       </c>
       <c r="H252" t="s">
-        <v>330</v>
+        <v>62</v>
       </c>
       <c r="I252" t="s">
         <v>8</v>
       </c>
       <c r="L252" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="M252" t="s">
         <v>64</v>
@@ -7409,7 +7415,7 @@
         <v>8</v>
       </c>
       <c r="L253" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="M253" t="s">
         <v>241</v>
@@ -7435,10 +7441,10 @@
         <v>8</v>
       </c>
       <c r="L254" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="M254" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="255" spans="1:13">
@@ -7449,10 +7455,10 @@
         <v>8</v>
       </c>
       <c r="L255" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="M255" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="256" spans="1:13">
@@ -7484,10 +7490,10 @@
         <v>8</v>
       </c>
       <c r="L256" t="s">
+        <v>407</v>
+      </c>
+      <c r="M256" t="s">
         <v>406</v>
-      </c>
-      <c r="M256" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="257" spans="1:13">
@@ -7495,7 +7501,7 @@
         <v>14</v>
       </c>
       <c r="L257" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M257" t="s">
         <v>158</v>
@@ -7506,7 +7512,7 @@
         <v>14</v>
       </c>
       <c r="L258" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="M258" t="s">
         <v>158</v>
@@ -7517,16 +7523,16 @@
         <v>3</v>
       </c>
       <c r="H259" t="s">
-        <v>24</v>
+        <v>313</v>
       </c>
       <c r="I259" t="s">
         <v>8</v>
       </c>
       <c r="L259" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="M259" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="260" spans="1:13">
@@ -7558,10 +7564,10 @@
         <v>8</v>
       </c>
       <c r="L260" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="M260" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="261" spans="1:13">
@@ -7572,10 +7578,10 @@
         <v>8</v>
       </c>
       <c r="L261" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="M261" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="262" spans="1:13">
@@ -7607,7 +7613,7 @@
         <v>8</v>
       </c>
       <c r="L262" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="M262" t="s">
         <v>117</v>
@@ -7621,10 +7627,10 @@
         <v>8</v>
       </c>
       <c r="L263" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="M263" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="264" spans="1:13">
@@ -7641,7 +7647,7 @@
         <v>30</v>
       </c>
       <c r="L264" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="M264" t="s">
         <v>92</v>
@@ -7676,10 +7682,10 @@
         <v>8</v>
       </c>
       <c r="L265" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="M265" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="266" spans="1:13">
@@ -7690,10 +7696,10 @@
         <v>8</v>
       </c>
       <c r="L266" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="M266" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="267" spans="1:13">
@@ -7725,10 +7731,10 @@
         <v>8</v>
       </c>
       <c r="L267" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="M267" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="268" spans="1:13">
@@ -7760,10 +7766,10 @@
         <v>8</v>
       </c>
       <c r="L268" t="s">
+        <v>424</v>
+      </c>
+      <c r="M268" t="s">
         <v>423</v>
-      </c>
-      <c r="M268" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="269" spans="1:13">
@@ -7774,10 +7780,10 @@
         <v>8</v>
       </c>
       <c r="L269" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="M269" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="270" spans="1:13">
@@ -7788,10 +7794,10 @@
         <v>8</v>
       </c>
       <c r="L270" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="M270" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="271" spans="1:13">
@@ -7823,10 +7829,10 @@
         <v>8</v>
       </c>
       <c r="L271" t="s">
+        <v>428</v>
+      </c>
+      <c r="M271" t="s">
         <v>427</v>
-      </c>
-      <c r="M271" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="272" spans="1:13">
@@ -7840,7 +7846,7 @@
         <v>8</v>
       </c>
       <c r="L272" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="M272" t="s">
         <v>133</v>
@@ -7875,10 +7881,10 @@
         <v>8</v>
       </c>
       <c r="L273" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="M273" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="274" spans="1:13">
@@ -7886,7 +7892,7 @@
         <v>3</v>
       </c>
       <c r="H274" t="s">
-        <v>431</v>
+        <v>24</v>
       </c>
       <c r="I274" t="s">
         <v>8</v>
@@ -8404,7 +8410,7 @@
         <v>6</v>
       </c>
       <c r="H293" t="s">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="I293" t="s">
         <v>8</v>
@@ -8413,7 +8419,7 @@
         <v>462</v>
       </c>
       <c r="M293" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="294" spans="1:13">
@@ -8421,7 +8427,7 @@
         <v>3</v>
       </c>
       <c r="H294" t="s">
-        <v>149</v>
+        <v>85</v>
       </c>
       <c r="I294" t="s">
         <v>8</v>
@@ -8430,7 +8436,7 @@
         <v>463</v>
       </c>
       <c r="M294" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="295" spans="1:13">
@@ -8675,7 +8681,7 @@
         <v>478</v>
       </c>
       <c r="M304" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="305" spans="1:13">
@@ -8710,7 +8716,7 @@
         <v>479</v>
       </c>
       <c r="M305" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="306" spans="1:13">
@@ -8727,7 +8733,7 @@
         <v>3</v>
       </c>
       <c r="H306" t="s">
-        <v>24</v>
+        <v>143</v>
       </c>
       <c r="I306" t="s">
         <v>8</v>
@@ -9003,7 +9009,7 @@
         <v>3</v>
       </c>
       <c r="H318" t="s">
-        <v>24</v>
+        <v>313</v>
       </c>
       <c r="I318" t="s">
         <v>8</v>
@@ -9012,7 +9018,7 @@
         <v>496</v>
       </c>
       <c r="M318" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="319" spans="1:13">
@@ -9392,7 +9398,7 @@
         <v>6</v>
       </c>
       <c r="H334" t="s">
-        <v>431</v>
+        <v>24</v>
       </c>
       <c r="I334" t="s">
         <v>8</v>

</xml_diff>